<commit_message>
update get course that can handle get all courses and get it by id
</commit_message>
<xml_diff>
--- a/public/uploads/QueryOptimizationTutorial.xlsx
+++ b/public/uploads/QueryOptimizationTutorial.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\Y3\T2\ADV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\Y3\T2\SE_Project\project_se_t12\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A47A9E-5BD6-4419-966C-72A766C91975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FD2F8D-7710-4ED2-9003-75A6F5821953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D8E702ED-52D4-4C86-A569-159188F4AE1B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Invoice</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t xml:space="preserve">Search for Customer : </t>
+  </si>
+  <si>
+    <t>Hello</t>
   </si>
 </sst>
 </file>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F955776-2471-498E-BAAD-85BADF44F42A}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -898,6 +901,11 @@
         <v>259144</v>
       </c>
     </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
delete course_student and when delete course the file that relate to that course is deleted too, add Update, delete, and get for student
</commit_message>
<xml_diff>
--- a/public/uploads/QueryOptimizationTutorial.xlsx
+++ b/public/uploads/QueryOptimizationTutorial.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\Y3\T2\SE_Project\project_se_t12\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU\Y3\T2\ADV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FD2F8D-7710-4ED2-9003-75A6F5821953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A47A9E-5BD6-4419-966C-72A766C91975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D8E702ED-52D4-4C86-A569-159188F4AE1B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Invoice</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t xml:space="preserve">Search for Customer : </t>
-  </si>
-  <si>
-    <t>Hello</t>
   </si>
 </sst>
 </file>
@@ -522,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F955776-2471-498E-BAAD-85BADF44F42A}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -901,11 +898,6 @@
         <v>259144</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>